<commit_message>
mas cambios --> parar cuando cambia la info del excel de records a historico de maarcas
</commit_message>
<xml_diff>
--- a/projectSimilarToTennisOne/Resources/Temp/ExcelRecordsFiles/recordsClub__Listado_de_Marcas p50.xlsx
+++ b/projectSimilarToTennisOne/Resources/Temp/ExcelRecordsFiles/recordsClub__Listado_de_Marcas p50.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clubdetenis-my.sharepoint.com/personal/imanol_club-tenis_com/Documents/2. Equipo/Marcas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\Downloads\recordsNatacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{1D1638F9-F5D9-4AFB-AB40-A1CEBDA4132F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19C031DC-2A75-454B-AF3E-656C47F08806}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5211BE7F-3E63-4E46-B9E2-76000410F2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4545" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="p50m" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">p50m!$A$1:$J$1948</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -5933,10 +5936,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -6256,8 +6255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1948"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A1930" workbookViewId="0">
+      <selection activeCell="D1915" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68611,6 +68610,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J1948" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>